<commit_message>
raw_state no longer normalized before calculating metrics
</commit_message>
<xml_diff>
--- a/to_edit.xlsx
+++ b/to_edit.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\Documents\Github\DMRG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6ED47886-3EF8-4142-B2A4-E193154C5693}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E2B40E-8454-495E-B353-6D99492540D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="to_edit" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -671,146 +671,302 @@
               <c:f>to_edit!$A$2:$A$1533</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="47"/>
+                <c:ptCount val="99"/>
                 <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="23">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="24">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="25">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="26">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="27">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="28">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="29">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="30">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="31">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="32">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="55">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="56">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="57">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="58">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="59">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="60">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="61">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="62">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="63">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="64">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="65">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="29">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="66">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="88">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="89">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="90">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="91">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="92">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="93">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="94">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="95">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="96">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="97">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="98">
                   <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
@@ -821,146 +977,302 @@
               <c:f>to_edit!$E$2:$E$1533</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="47"/>
+                <c:ptCount val="99"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.99998642604911503</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.99996654114410299</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.99997257760175295</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99997105597215696</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.99997070841917701</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.99997297283883202</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.99997115982635698</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.999972316202828</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.99997137878736497</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.99997158583724899</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99997111002957595</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>0.99999911377204698</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="23">
                   <c:v>0.99999247230298205</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="24">
                   <c:v>0.99999699767054295</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="25">
                   <c:v>0.99999637367194805</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="26">
                   <c:v>0.99999685722158205</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="27">
                   <c:v>0.999996869204545</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="28">
                   <c:v>0.999996759396517</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="29">
                   <c:v>0.99999649060296802</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="30">
                   <c:v>0.999996386388601</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="31">
                   <c:v>0.99999652083944102</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="32">
                   <c:v>0.99999645959347805</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.99999691640899002</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.99999627549041004</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.99999628224900095</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.99999617212812197</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.99999661692337605</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.99999674716137299</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.99999671988225403</c:v>
-                </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="33">
+                  <c:v>0.99999811142033301</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.99999621913184</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.99999728794862097</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.99999740761590805</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.99999697464913795</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.99999709532930103</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.99999724632259201</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.99999716510212899</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.99999728494072904</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.99999627247008405</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.99999660207298902</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.99999788051122196</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.99999699759517302</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.99999831580410103</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.99999762604970799</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.99999759443424596</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.99999797479169905</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.99999738229059998</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.99999818224530301</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.99999813613954402</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.99999812089218698</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.99999787468540802</c:v>
+                </c:pt>
+                <c:pt idx="55">
                   <c:v>0.999998243768491</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="56">
                   <c:v>0.99999653825256996</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="57">
                   <c:v>0.99999786451103601</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="58">
                   <c:v>0.99999746101283005</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="59">
                   <c:v>0.99999815995596897</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="60">
                   <c:v>0.99999739493779305</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="61">
                   <c:v>0.99999742533298197</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="62">
                   <c:v>0.99999741933337005</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="63">
                   <c:v>0.99999729347272504</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="64">
                   <c:v>0.999997651879734</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="65">
                   <c:v>0.99999696279261296</c:v>
                 </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.99999667680301796</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.999997468090282</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.99999779028034996</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.99999775362190102</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.99999801901466001</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.99999789849971998</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.99999767936970396</c:v>
-                </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="66">
+                  <c:v>0.99996371882169</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.99996880147084999</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.99998118124759094</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.99997073977371598</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.99996592039175802</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.99997317176409795</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.99997746468717996</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.99997681270977001</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.99997918800187102</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.999977615788333</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.99997721089381497</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.99998933561828296</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.99998766401226502</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.99998848016004405</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.99999034922841101</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.99998982744986498</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.999990547109182</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.99999199443572795</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.999992781697987</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.99999180477713701</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.99999104622073798</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.99999011039447405</c:v>
+                </c:pt>
+                <c:pt idx="88">
                   <c:v>0.99989629000041802</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="89">
                   <c:v>0.99986539278511799</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="90">
                   <c:v>0.99987343275057505</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="91">
                   <c:v>0.99985003856653298</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="92">
                   <c:v>0.99989900418964395</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="93">
                   <c:v>0.99991414976578297</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="94">
                   <c:v>0.99987617879721002</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="95">
                   <c:v>0.99990742412824996</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="96">
                   <c:v>0.99984867173346303</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="97">
                   <c:v>0.99991062521199603</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="98">
                   <c:v>0.99988798501262</c:v>
                 </c:pt>
               </c:numCache>
@@ -1025,7 +1337,7 @@
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="47"/>
+                      <c:ptCount val="99"/>
                       <c:pt idx="0">
                         <c:v>20</c:v>
                       </c:pt>
@@ -1167,6 +1479,162 @@
                       <c:pt idx="46">
                         <c:v>20</c:v>
                       </c:pt>
+                      <c:pt idx="47">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="65">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="66">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="67">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="68">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="69">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="70">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="72">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="73">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="74">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="75">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="76">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="77">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="78">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="79">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="80">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="81">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="82">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="83">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="84">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="85">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="86">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="87">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="88">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="89">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="90">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="91">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="92">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="93">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="94">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="95">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="96">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="97">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="98">
+                        <c:v>20</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:xVal>
@@ -1181,146 +1649,302 @@
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="47"/>
+                      <c:ptCount val="99"/>
                       <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.99998642604911503</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.99996654114410299</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.99997257760175295</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.99997105597215696</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.99997070841917701</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.99997297283883202</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.99997115982635698</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0.999972316202828</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>0.99997137878736497</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>0.99997158583724899</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>0.99997111002957595</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
                         <c:v>0.99999911377204698</c:v>
                       </c:pt>
-                      <c:pt idx="1">
+                      <c:pt idx="23">
                         <c:v>0.99999247230298205</c:v>
                       </c:pt>
-                      <c:pt idx="2">
+                      <c:pt idx="24">
                         <c:v>0.99999699767054295</c:v>
                       </c:pt>
-                      <c:pt idx="3">
+                      <c:pt idx="25">
                         <c:v>0.99999637367194805</c:v>
                       </c:pt>
-                      <c:pt idx="4">
+                      <c:pt idx="26">
                         <c:v>0.99999685722158205</c:v>
                       </c:pt>
-                      <c:pt idx="5">
+                      <c:pt idx="27">
                         <c:v>0.999996869204545</c:v>
                       </c:pt>
-                      <c:pt idx="6">
+                      <c:pt idx="28">
                         <c:v>0.999996759396517</c:v>
                       </c:pt>
-                      <c:pt idx="7">
+                      <c:pt idx="29">
                         <c:v>0.99999649060296802</c:v>
                       </c:pt>
-                      <c:pt idx="8">
+                      <c:pt idx="30">
                         <c:v>0.999996386388601</c:v>
                       </c:pt>
-                      <c:pt idx="9">
+                      <c:pt idx="31">
                         <c:v>0.99999652083944102</c:v>
                       </c:pt>
-                      <c:pt idx="10">
+                      <c:pt idx="32">
                         <c:v>0.99999645959347805</c:v>
                       </c:pt>
-                      <c:pt idx="11">
-                        <c:v>0.99999691640899002</c:v>
+                      <c:pt idx="33">
+                        <c:v>0.99999811142033301</c:v>
                       </c:pt>
-                      <c:pt idx="12">
-                        <c:v>0.99999627549041004</c:v>
+                      <c:pt idx="34">
+                        <c:v>0.99999621913184</c:v>
                       </c:pt>
-                      <c:pt idx="13">
-                        <c:v>0.99999628224900095</c:v>
+                      <c:pt idx="35">
+                        <c:v>0.99999728794862097</c:v>
                       </c:pt>
-                      <c:pt idx="14">
-                        <c:v>0.99999617212812197</c:v>
+                      <c:pt idx="36">
+                        <c:v>0.99999740761590805</c:v>
                       </c:pt>
-                      <c:pt idx="15">
-                        <c:v>0.99999661692337605</c:v>
+                      <c:pt idx="37">
+                        <c:v>0.99999697464913795</c:v>
                       </c:pt>
-                      <c:pt idx="16">
-                        <c:v>0.99999674716137299</c:v>
+                      <c:pt idx="38">
+                        <c:v>0.99999709532930103</c:v>
                       </c:pt>
-                      <c:pt idx="17">
-                        <c:v>0.99999671988225403</c:v>
+                      <c:pt idx="39">
+                        <c:v>0.99999724632259201</c:v>
                       </c:pt>
-                      <c:pt idx="18">
+                      <c:pt idx="40">
+                        <c:v>0.99999716510212899</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>0.99999728494072904</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>0.99999627247008405</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>0.99999660207298902</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>0.99999788051122196</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>0.99999699759517302</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>0.99999831580410103</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>0.99999762604970799</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>0.99999759443424596</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>0.99999797479169905</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>0.99999738229059998</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>0.99999818224530301</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>0.99999813613954402</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>0.99999812089218698</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>0.99999787468540802</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
                         <c:v>0.999998243768491</c:v>
                       </c:pt>
-                      <c:pt idx="19">
+                      <c:pt idx="56">
                         <c:v>0.99999653825256996</c:v>
                       </c:pt>
-                      <c:pt idx="20">
+                      <c:pt idx="57">
                         <c:v>0.99999786451103601</c:v>
                       </c:pt>
-                      <c:pt idx="21">
+                      <c:pt idx="58">
                         <c:v>0.99999746101283005</c:v>
                       </c:pt>
-                      <c:pt idx="22">
+                      <c:pt idx="59">
                         <c:v>0.99999815995596897</c:v>
                       </c:pt>
-                      <c:pt idx="23">
+                      <c:pt idx="60">
                         <c:v>0.99999739493779305</c:v>
                       </c:pt>
-                      <c:pt idx="24">
+                      <c:pt idx="61">
                         <c:v>0.99999742533298197</c:v>
                       </c:pt>
-                      <c:pt idx="25">
+                      <c:pt idx="62">
                         <c:v>0.99999741933337005</c:v>
                       </c:pt>
-                      <c:pt idx="26">
+                      <c:pt idx="63">
                         <c:v>0.99999729347272504</c:v>
                       </c:pt>
-                      <c:pt idx="27">
+                      <c:pt idx="64">
                         <c:v>0.999997651879734</c:v>
                       </c:pt>
-                      <c:pt idx="28">
+                      <c:pt idx="65">
                         <c:v>0.99999696279261296</c:v>
                       </c:pt>
-                      <c:pt idx="29">
-                        <c:v>0.99999667680301796</c:v>
+                      <c:pt idx="66">
+                        <c:v>0.99996371882169</c:v>
                       </c:pt>
-                      <c:pt idx="30">
-                        <c:v>0.999997468090282</c:v>
+                      <c:pt idx="67">
+                        <c:v>0.99996880147084999</c:v>
                       </c:pt>
-                      <c:pt idx="31">
-                        <c:v>0.99999779028034996</c:v>
+                      <c:pt idx="68">
+                        <c:v>0.99998118124759094</c:v>
                       </c:pt>
-                      <c:pt idx="32">
-                        <c:v>0.99999775362190102</c:v>
+                      <c:pt idx="69">
+                        <c:v>0.99997073977371598</c:v>
                       </c:pt>
-                      <c:pt idx="33">
-                        <c:v>0.99999801901466001</c:v>
+                      <c:pt idx="70">
+                        <c:v>0.99996592039175802</c:v>
                       </c:pt>
-                      <c:pt idx="34">
-                        <c:v>0.99999789849971998</c:v>
+                      <c:pt idx="71">
+                        <c:v>0.99997317176409795</c:v>
                       </c:pt>
-                      <c:pt idx="35">
-                        <c:v>0.99999767936970396</c:v>
+                      <c:pt idx="72">
+                        <c:v>0.99997746468717996</c:v>
                       </c:pt>
-                      <c:pt idx="36">
+                      <c:pt idx="73">
+                        <c:v>0.99997681270977001</c:v>
+                      </c:pt>
+                      <c:pt idx="74">
+                        <c:v>0.99997918800187102</c:v>
+                      </c:pt>
+                      <c:pt idx="75">
+                        <c:v>0.999977615788333</c:v>
+                      </c:pt>
+                      <c:pt idx="76">
+                        <c:v>0.99997721089381497</c:v>
+                      </c:pt>
+                      <c:pt idx="77">
+                        <c:v>0.99998933561828296</c:v>
+                      </c:pt>
+                      <c:pt idx="78">
+                        <c:v>0.99998766401226502</c:v>
+                      </c:pt>
+                      <c:pt idx="79">
+                        <c:v>0.99998848016004405</c:v>
+                      </c:pt>
+                      <c:pt idx="80">
+                        <c:v>0.99999034922841101</c:v>
+                      </c:pt>
+                      <c:pt idx="81">
+                        <c:v>0.99998982744986498</c:v>
+                      </c:pt>
+                      <c:pt idx="82">
+                        <c:v>0.999990547109182</c:v>
+                      </c:pt>
+                      <c:pt idx="83">
+                        <c:v>0.99999199443572795</c:v>
+                      </c:pt>
+                      <c:pt idx="84">
+                        <c:v>0.999992781697987</c:v>
+                      </c:pt>
+                      <c:pt idx="85">
+                        <c:v>0.99999180477713701</c:v>
+                      </c:pt>
+                      <c:pt idx="86">
+                        <c:v>0.99999104622073798</c:v>
+                      </c:pt>
+                      <c:pt idx="87">
+                        <c:v>0.99999011039447405</c:v>
+                      </c:pt>
+                      <c:pt idx="88">
                         <c:v>0.99989629000041802</c:v>
                       </c:pt>
-                      <c:pt idx="37">
+                      <c:pt idx="89">
                         <c:v>0.99986539278511799</c:v>
                       </c:pt>
-                      <c:pt idx="38">
+                      <c:pt idx="90">
                         <c:v>0.99987343275057505</c:v>
                       </c:pt>
-                      <c:pt idx="39">
+                      <c:pt idx="91">
                         <c:v>0.99985003856653298</c:v>
                       </c:pt>
-                      <c:pt idx="40">
+                      <c:pt idx="92">
                         <c:v>0.99989900418964395</c:v>
                       </c:pt>
-                      <c:pt idx="41">
+                      <c:pt idx="93">
                         <c:v>0.99991414976578297</c:v>
                       </c:pt>
-                      <c:pt idx="42">
+                      <c:pt idx="94">
                         <c:v>0.99987617879721002</c:v>
                       </c:pt>
-                      <c:pt idx="43">
+                      <c:pt idx="95">
                         <c:v>0.99990742412824996</c:v>
                       </c:pt>
-                      <c:pt idx="44">
+                      <c:pt idx="96">
                         <c:v>0.99984867173346303</c:v>
                       </c:pt>
-                      <c:pt idx="45">
+                      <c:pt idx="97">
                         <c:v>0.99991062521199603</c:v>
                       </c:pt>
-                      <c:pt idx="46">
+                      <c:pt idx="98">
                         <c:v>0.99988798501262</c:v>
                       </c:pt>
                     </c:numCache>
@@ -1365,7 +1989,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>to_edit!$A$2:$A$1533</c15:sqref>
@@ -1374,146 +1998,302 @@
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="47"/>
+                      <c:ptCount val="99"/>
                       <c:pt idx="0">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
                         <c:v>5</c:v>
                       </c:pt>
-                      <c:pt idx="1">
+                      <c:pt idx="23">
                         <c:v>5</c:v>
                       </c:pt>
-                      <c:pt idx="2">
+                      <c:pt idx="24">
                         <c:v>5</c:v>
                       </c:pt>
-                      <c:pt idx="3">
+                      <c:pt idx="25">
                         <c:v>5</c:v>
                       </c:pt>
-                      <c:pt idx="4">
+                      <c:pt idx="26">
                         <c:v>5</c:v>
                       </c:pt>
-                      <c:pt idx="5">
+                      <c:pt idx="27">
                         <c:v>5</c:v>
                       </c:pt>
-                      <c:pt idx="6">
+                      <c:pt idx="28">
                         <c:v>5</c:v>
                       </c:pt>
-                      <c:pt idx="7">
+                      <c:pt idx="29">
                         <c:v>5</c:v>
                       </c:pt>
-                      <c:pt idx="8">
+                      <c:pt idx="30">
                         <c:v>5</c:v>
                       </c:pt>
-                      <c:pt idx="9">
+                      <c:pt idx="31">
                         <c:v>5</c:v>
                       </c:pt>
-                      <c:pt idx="10">
+                      <c:pt idx="32">
                         <c:v>5</c:v>
                       </c:pt>
-                      <c:pt idx="11">
-                        <c:v>5</c:v>
+                      <c:pt idx="33">
+                        <c:v>6</c:v>
                       </c:pt>
-                      <c:pt idx="12">
-                        <c:v>5</c:v>
+                      <c:pt idx="34">
+                        <c:v>6</c:v>
                       </c:pt>
-                      <c:pt idx="13">
-                        <c:v>5</c:v>
+                      <c:pt idx="35">
+                        <c:v>6</c:v>
                       </c:pt>
-                      <c:pt idx="14">
-                        <c:v>5</c:v>
+                      <c:pt idx="36">
+                        <c:v>6</c:v>
                       </c:pt>
-                      <c:pt idx="15">
-                        <c:v>5</c:v>
+                      <c:pt idx="37">
+                        <c:v>6</c:v>
                       </c:pt>
-                      <c:pt idx="16">
-                        <c:v>5</c:v>
+                      <c:pt idx="38">
+                        <c:v>6</c:v>
                       </c:pt>
-                      <c:pt idx="17">
-                        <c:v>5</c:v>
+                      <c:pt idx="39">
+                        <c:v>6</c:v>
                       </c:pt>
-                      <c:pt idx="18">
+                      <c:pt idx="40">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="19">
+                      <c:pt idx="56">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="20">
+                      <c:pt idx="57">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="21">
+                      <c:pt idx="58">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="22">
+                      <c:pt idx="59">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="23">
+                      <c:pt idx="60">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="24">
+                      <c:pt idx="61">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="25">
+                      <c:pt idx="62">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="26">
+                      <c:pt idx="63">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="27">
+                      <c:pt idx="64">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="28">
+                      <c:pt idx="65">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="29">
-                        <c:v>8</c:v>
+                      <c:pt idx="66">
+                        <c:v>9</c:v>
                       </c:pt>
-                      <c:pt idx="30">
-                        <c:v>8</c:v>
+                      <c:pt idx="67">
+                        <c:v>9</c:v>
                       </c:pt>
-                      <c:pt idx="31">
-                        <c:v>8</c:v>
+                      <c:pt idx="68">
+                        <c:v>9</c:v>
                       </c:pt>
-                      <c:pt idx="32">
-                        <c:v>8</c:v>
+                      <c:pt idx="69">
+                        <c:v>9</c:v>
                       </c:pt>
-                      <c:pt idx="33">
-                        <c:v>8</c:v>
+                      <c:pt idx="70">
+                        <c:v>9</c:v>
                       </c:pt>
-                      <c:pt idx="34">
-                        <c:v>8</c:v>
+                      <c:pt idx="71">
+                        <c:v>9</c:v>
                       </c:pt>
-                      <c:pt idx="35">
-                        <c:v>8</c:v>
+                      <c:pt idx="72">
+                        <c:v>9</c:v>
                       </c:pt>
-                      <c:pt idx="36">
+                      <c:pt idx="73">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="74">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="75">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="76">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="77">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="78">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="79">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="80">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="81">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="82">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="83">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="84">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="85">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="86">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="87">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="88">
                         <c:v>11</c:v>
                       </c:pt>
-                      <c:pt idx="37">
+                      <c:pt idx="89">
                         <c:v>11</c:v>
                       </c:pt>
-                      <c:pt idx="38">
+                      <c:pt idx="90">
                         <c:v>11</c:v>
                       </c:pt>
-                      <c:pt idx="39">
+                      <c:pt idx="91">
                         <c:v>11</c:v>
                       </c:pt>
-                      <c:pt idx="40">
+                      <c:pt idx="92">
                         <c:v>11</c:v>
                       </c:pt>
-                      <c:pt idx="41">
+                      <c:pt idx="93">
                         <c:v>11</c:v>
                       </c:pt>
-                      <c:pt idx="42">
+                      <c:pt idx="94">
                         <c:v>11</c:v>
                       </c:pt>
-                      <c:pt idx="43">
+                      <c:pt idx="95">
                         <c:v>11</c:v>
                       </c:pt>
-                      <c:pt idx="44">
+                      <c:pt idx="96">
                         <c:v>11</c:v>
                       </c:pt>
-                      <c:pt idx="45">
+                      <c:pt idx="97">
                         <c:v>11</c:v>
                       </c:pt>
-                      <c:pt idx="46">
+                      <c:pt idx="98">
                         <c:v>11</c:v>
                       </c:pt>
                     </c:numCache>
@@ -1521,7 +2301,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>to_edit!$D$2:$D$1533</c15:sqref>
@@ -1530,153 +2310,309 @@
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="47"/>
+                      <c:ptCount val="99"/>
                       <c:pt idx="0">
+                        <c:v>0.999999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.999999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.999999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.999999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.999999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.999999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.999999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.999999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.999999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.999999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.999999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.99997373835133097</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.99988854573173103</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.99995402056217997</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.99995375954985499</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.99994757882104002</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.99995101329024605</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.99995192678035005</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0.999954715230436</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>0.99995480289777605</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>0.99995305254191402</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>0.99995330788567405</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
                         <c:v>0.99999461034390102</c:v>
                       </c:pt>
-                      <c:pt idx="1">
+                      <c:pt idx="23">
                         <c:v>0.99998038656231802</c:v>
                       </c:pt>
-                      <c:pt idx="2">
+                      <c:pt idx="24">
                         <c:v>0.99999061822672997</c:v>
                       </c:pt>
-                      <c:pt idx="3">
+                      <c:pt idx="25">
                         <c:v>0.99999065682163102</c:v>
                       </c:pt>
-                      <c:pt idx="4">
+                      <c:pt idx="26">
                         <c:v>0.999990872952494</c:v>
                       </c:pt>
-                      <c:pt idx="5">
+                      <c:pt idx="27">
                         <c:v>0.99999188665735605</c:v>
                       </c:pt>
-                      <c:pt idx="6">
+                      <c:pt idx="28">
                         <c:v>0.99999088497914701</c:v>
                       </c:pt>
-                      <c:pt idx="7">
+                      <c:pt idx="29">
                         <c:v>0.99999176876111695</c:v>
                       </c:pt>
-                      <c:pt idx="8">
+                      <c:pt idx="30">
                         <c:v>0.99999186765923498</c:v>
                       </c:pt>
-                      <c:pt idx="9">
+                      <c:pt idx="31">
                         <c:v>0.99999228460179201</c:v>
                       </c:pt>
-                      <c:pt idx="10">
+                      <c:pt idx="32">
                         <c:v>0.99999167887589202</c:v>
                       </c:pt>
-                      <c:pt idx="11">
-                        <c:v>0.99999173386144502</c:v>
+                      <c:pt idx="33">
+                        <c:v>0.99998324102973402</c:v>
                       </c:pt>
-                      <c:pt idx="12">
-                        <c:v>0.99999220502029695</c:v>
+                      <c:pt idx="34">
+                        <c:v>0.99999193810143905</c:v>
                       </c:pt>
-                      <c:pt idx="13">
-                        <c:v>0.99999228280252705</c:v>
+                      <c:pt idx="35">
+                        <c:v>0.99998877997513402</c:v>
                       </c:pt>
-                      <c:pt idx="14">
-                        <c:v>0.99999234835366502</c:v>
+                      <c:pt idx="36">
+                        <c:v>0.99998315029649998</c:v>
                       </c:pt>
-                      <c:pt idx="15">
-                        <c:v>0.99999194448764905</c:v>
+                      <c:pt idx="37">
+                        <c:v>0.99998688731490004</c:v>
                       </c:pt>
-                      <c:pt idx="16">
-                        <c:v>0.99999233666585996</c:v>
+                      <c:pt idx="38">
+                        <c:v>0.99998686594110098</c:v>
                       </c:pt>
-                      <c:pt idx="17">
-                        <c:v>0.99999242473976202</c:v>
+                      <c:pt idx="39">
+                        <c:v>0.99998182482192499</c:v>
                       </c:pt>
-                      <c:pt idx="18">
+                      <c:pt idx="40">
+                        <c:v>0.999975527814564</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>0.99998199249872299</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>0.99998196758593505</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>0.99998212786546603</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>0.99999363455062495</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>0.99980585439059</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>0.99998968097238405</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>0.99998587631454205</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>0.99999065504271301</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>0.99998853592826498</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>0.99999078524853702</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>0.99999298634849598</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>0.99999149395473996</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>0.99999462581880805</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>0.99999004647107304</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
                         <c:v>0.99999240085052699</c:v>
                       </c:pt>
-                      <c:pt idx="19">
+                      <c:pt idx="56">
                         <c:v>0.99998329637641903</c:v>
                       </c:pt>
-                      <c:pt idx="20">
+                      <c:pt idx="57">
                         <c:v>0.99999338285903705</c:v>
                       </c:pt>
-                      <c:pt idx="21">
+                      <c:pt idx="58">
                         <c:v>0.999993092896997</c:v>
                       </c:pt>
-                      <c:pt idx="22">
+                      <c:pt idx="59">
                         <c:v>0.99999363520697004</c:v>
                       </c:pt>
-                      <c:pt idx="23">
+                      <c:pt idx="60">
                         <c:v>0.99999374946684605</c:v>
                       </c:pt>
-                      <c:pt idx="24">
+                      <c:pt idx="61">
                         <c:v>0.99999487345498095</c:v>
                       </c:pt>
-                      <c:pt idx="25">
+                      <c:pt idx="62">
                         <c:v>0.99999102887352798</c:v>
                       </c:pt>
-                      <c:pt idx="26">
+                      <c:pt idx="63">
                         <c:v>0.99999162626375804</c:v>
                       </c:pt>
-                      <c:pt idx="27">
+                      <c:pt idx="64">
                         <c:v>0.99999383140106601</c:v>
                       </c:pt>
-                      <c:pt idx="28">
+                      <c:pt idx="65">
                         <c:v>0.99999354618847502</c:v>
                       </c:pt>
-                      <c:pt idx="29">
-                        <c:v>0.99999387149672103</c:v>
+                      <c:pt idx="66">
+                        <c:v>0.99992583006380897</c:v>
                       </c:pt>
-                      <c:pt idx="30">
-                        <c:v>0.99999520760600003</c:v>
+                      <c:pt idx="67">
+                        <c:v>0.99975076316179501</c:v>
                       </c:pt>
-                      <c:pt idx="31">
-                        <c:v>0.99999192596888098</c:v>
+                      <c:pt idx="68">
+                        <c:v>0.99985933209399502</c:v>
                       </c:pt>
-                      <c:pt idx="32">
-                        <c:v>0.99999447733200897</c:v>
+                      <c:pt idx="69">
+                        <c:v>0.99986209171189599</c:v>
                       </c:pt>
-                      <c:pt idx="33">
-                        <c:v>0.99999429498918302</c:v>
+                      <c:pt idx="70">
+                        <c:v>0.99991076694152703</c:v>
                       </c:pt>
-                      <c:pt idx="34">
-                        <c:v>0.99999445981671697</c:v>
+                      <c:pt idx="71">
+                        <c:v>0.99991237247253295</c:v>
                       </c:pt>
-                      <c:pt idx="35">
-                        <c:v>0.99999311855357997</c:v>
+                      <c:pt idx="72">
+                        <c:v>0.99991727747706205</c:v>
                       </c:pt>
-                      <c:pt idx="36">
+                      <c:pt idx="73">
+                        <c:v>0.99993983705332601</c:v>
+                      </c:pt>
+                      <c:pt idx="74">
+                        <c:v>0.99991503038091101</c:v>
+                      </c:pt>
+                      <c:pt idx="75">
+                        <c:v>0.99992716973571705</c:v>
+                      </c:pt>
+                      <c:pt idx="76">
+                        <c:v>0.99992507878511205</c:v>
+                      </c:pt>
+                      <c:pt idx="77">
+                        <c:v>0.99998133638754205</c:v>
+                      </c:pt>
+                      <c:pt idx="78">
+                        <c:v>0.99286634034870702</c:v>
+                      </c:pt>
+                      <c:pt idx="79">
+                        <c:v>0.99997299575218701</c:v>
+                      </c:pt>
+                      <c:pt idx="80">
+                        <c:v>0.99997448928464805</c:v>
+                      </c:pt>
+                      <c:pt idx="81">
+                        <c:v>0.99997530554168801</c:v>
+                      </c:pt>
+                      <c:pt idx="82">
+                        <c:v>0.99997345511786995</c:v>
+                      </c:pt>
+                      <c:pt idx="83">
+                        <c:v>0.99996687210318402</c:v>
+                      </c:pt>
+                      <c:pt idx="84">
+                        <c:v>0.999966373066002</c:v>
+                      </c:pt>
+                      <c:pt idx="85">
+                        <c:v>0.99996919643281101</c:v>
+                      </c:pt>
+                      <c:pt idx="86">
+                        <c:v>0.99996587016420402</c:v>
+                      </c:pt>
+                      <c:pt idx="87">
+                        <c:v>0.99996217352355998</c:v>
+                      </c:pt>
+                      <c:pt idx="88">
                         <c:v>0.96052589004384104</c:v>
                       </c:pt>
-                      <c:pt idx="37">
+                      <c:pt idx="89">
                         <c:v>0.99074930651716198</c:v>
                       </c:pt>
-                      <c:pt idx="38">
+                      <c:pt idx="90">
                         <c:v>0.999614110876899</c:v>
                       </c:pt>
-                      <c:pt idx="39">
+                      <c:pt idx="91">
                         <c:v>0.99934149392382099</c:v>
                       </c:pt>
-                      <c:pt idx="40">
+                      <c:pt idx="92">
                         <c:v>0.99974354797837195</c:v>
                       </c:pt>
-                      <c:pt idx="41">
+                      <c:pt idx="93">
                         <c:v>0.99972095191935895</c:v>
                       </c:pt>
-                      <c:pt idx="42">
+                      <c:pt idx="94">
                         <c:v>0.99978445804804394</c:v>
                       </c:pt>
-                      <c:pt idx="43">
+                      <c:pt idx="95">
                         <c:v>0.99968947094254501</c:v>
                       </c:pt>
-                      <c:pt idx="44">
+                      <c:pt idx="96">
                         <c:v>0.99963947146725196</c:v>
                       </c:pt>
-                      <c:pt idx="45">
+                      <c:pt idx="97">
                         <c:v>0.99977729706179397</c:v>
                       </c:pt>
-                      <c:pt idx="46">
+                      <c:pt idx="98">
                         <c:v>0.99970259274772499</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-212C-46A3-809E-48143832B988}"/>
                   </c:ext>
@@ -1953,9 +2889,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.8668371488568667E-2"/>
+          <c:y val="4.4433370510860826E-2"/>
+          <c:w val="0.63928410396456303"/>
+          <c:h val="0.8593811124264874"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -1963,605 +2909,19 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Compressed Dim vs. Distance</c:v>
+            <c:v>N = 5, D = 20</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>to_edit!$C$1523:$C$1533</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>to_edit!$F$1523:$F$1533</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.28097725871023599</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.13601980357902199</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.77808971453667E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.6290662054568601E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.2647384909866598E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.3624058950226401E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.07625601482893E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.4921037597022199E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.6852505758270698E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.1104641110756599E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.4388819252905598E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9C57-47C5-8C6E-655CDE9F3DF0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Compressed Dim vs. Similarity</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>to_edit!$C$1523:$C$1533</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>to_edit!$D$1523:$D$1533</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.96052589004384104</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.99074930651716198</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.999614110876899</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.99934149392382099</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.99974354797837195</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.99972095191935895</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.99978445804804394</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.99968947094254501</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.99963947146725196</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.99977729706179397</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.99970259274772499</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-9C57-47C5-8C6E-655CDE9F3DF0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1937641088"/>
-        <c:axId val="1448502176"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1937641088"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Compressed</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="de-DE" baseline="0"/>
-                  <a:t> Dimension (d), N = 11, D = 20</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1448502176"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1448502176"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Value</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1937641088"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Compressed Dim vs. Distance (N = 5, D = 20)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -2658,29 +3018,19 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Compressed Dim vs. Distance (N = 11, D = 20)</c:v>
+            <c:v>N = 11, D=20</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -2777,29 +3127,19 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Compressed Dim vs. Distance (N = 8, D = 20)</c:v>
+            <c:v>N=8, D=20</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -2889,6 +3229,777 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-4777-4AD0-AEF3-6F2C65267D9F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>N = 3, D = 20</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>to_edit!$C$155:$C$165</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>to_edit!$F$155:$F$172</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.1073424255447001E-8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3560804576936198E-8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1073424255447001E-8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3560804576936198E-8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1073424255447001E-8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3560804576936198E-8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3560804576936198E-8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1073424255447001E-8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5809568279517801E-8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1073424255447001E-8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.1073424255447001E-8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0404-45DE-B6BD-E8D28EE1AF8D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>N = 4, D = 20</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>to_edit!$C$326:$C$336</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>to_edit!$F$326:$F$336</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>7.2472958639114996E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.49301217858191E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.5895190516553999E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.6166990329388004E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.02392557307956E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.8981523280756399E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.8054290727978693E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.5168029889187104E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.5075866784903301E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.6899389148549404E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.6635515548324103E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0404-45DE-B6BD-E8D28EE1AF8D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>N = 6, D = 20</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>to_edit!$C$668:$C$678</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>to_edit!$F$669:$F$678</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4.0154448222407104E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.7370929619990499E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.8051190340211497E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1210711963011798E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1252431937142597E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0291256536376897E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.9960253624544496E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.0012500824331103E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.00539991414311E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.9786511075517104E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0404-45DE-B6BD-E8D28EE1AF8D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>N = 7</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>to_edit!$C$678:$C$849</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>to_edit!$F$839:$F$849</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3.5680385015490501E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.97051064148639E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5429126372972996E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.31482557720499E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.3231833842268599E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.7883341016640201E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.2929596931834003E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.7453041275311702E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.1245715555772201E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.2784695182214402E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.4617326066273104E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-0404-45DE-B6BD-E8D28EE1AF8D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>N = 8</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>to_edit!$C$1010:$C$1020</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>to_edit!$F$1010:$F$1020</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3.8984995759803799E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7799002724912502E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.63789526014572E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.71674669626739E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5678545459608001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.53568470125384E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.2020446647754801E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.2358296640476901E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0923675887401603E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.51243474917271E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.5927180583722098E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-0404-45DE-B6BD-E8D28EE1AF8D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>N = 9</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>to_edit!$C$1181:$C$1191</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>to_edit!$F$1181:$F$1191</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.2179485719180301E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.23265240557524E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.67730680560387E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.66077264009592E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.33591211144065E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3238393215739599E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.28625443002804E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.09693159927785E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.30360744927206E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.20689903706893E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.2241014246295199E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-0404-45DE-B6BD-E8D28EE1AF8D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:v>N = 10</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>to_edit!$C$1352:$C$1362</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>to_edit!$F$1352:$F$1362</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>6.1096010439767E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.119445884410425</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.3490472598969799E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.1429287204829196E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0277248541902098E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.2862723158686497E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.1397661903464501E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.2008455659494505E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.8490212369635801E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.2619411516950993E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.69787059475087E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-0404-45DE-B6BD-E8D28EE1AF8D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3048,8 +4159,14 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE"/>
-                  <a:t>Value</a:t>
+                  <a:t>Distance</a:t>
                 </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
               </a:p>
               <a:p>
                 <a:pPr>
@@ -3253,46 +4370,6 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4364,522 +5441,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4921,51 +5482,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>290512</xdr:colOff>
-      <xdr:row>510</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:colOff>312373</xdr:colOff>
+      <xdr:row>670</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>595312</xdr:colOff>
-      <xdr:row>1532</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{197C22D7-C960-4263-BC77-E047ADE5D78F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>478715</xdr:colOff>
-      <xdr:row>500</xdr:row>
-      <xdr:rowOff>6024</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>43</xdr:col>
-      <xdr:colOff>51953</xdr:colOff>
-      <xdr:row>1545</xdr:row>
-      <xdr:rowOff>103909</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>312965</xdr:colOff>
+      <xdr:row>1189</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4984,7 +5509,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5289,12 +5814,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G1533"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E1010" sqref="E1010"/>
+    <sheetView tabSelected="1" topLeftCell="A671" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L1359" sqref="L1359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8849,7 +9374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>3</v>
       </c>
@@ -8872,7 +9397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>3</v>
       </c>
@@ -8895,7 +9420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>3</v>
       </c>
@@ -8918,7 +9443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>3</v>
       </c>
@@ -8941,7 +9466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>3</v>
       </c>
@@ -8964,7 +9489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>3</v>
       </c>
@@ -8987,7 +9512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>3</v>
       </c>
@@ -9010,7 +9535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>3</v>
       </c>
@@ -9033,7 +9558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>3</v>
       </c>
@@ -9056,7 +9581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>3</v>
       </c>
@@ -9079,7 +9604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>3</v>
       </c>
@@ -12782,7 +13307,7 @@
         <v>2.6233264455214102E-3</v>
       </c>
     </row>
-    <row r="326" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>4</v>
       </c>
@@ -12805,7 +13330,7 @@
         <v>5.2103648404403201E-3</v>
       </c>
     </row>
-    <row r="327" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>4</v>
       </c>
@@ -12828,7 +13353,7 @@
         <v>8.1803246755186194E-3</v>
       </c>
     </row>
-    <row r="328" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>4</v>
       </c>
@@ -12851,7 +13376,7 @@
         <v>7.4057272765356598E-3</v>
       </c>
     </row>
-    <row r="329" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>4</v>
       </c>
@@ -12874,7 +13399,7 @@
         <v>7.60842005196032E-3</v>
       </c>
     </row>
-    <row r="330" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>4</v>
       </c>
@@ -12897,7 +13422,7 @@
         <v>7.6539637865747296E-3</v>
       </c>
     </row>
-    <row r="331" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>4</v>
       </c>
@@ -12920,7 +13445,7 @@
         <v>7.3521644660803302E-3</v>
       </c>
     </row>
-    <row r="332" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>4</v>
       </c>
@@ -12943,7 +13468,7 @@
         <v>7.5947578820477098E-3</v>
       </c>
     </row>
-    <row r="333" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>4</v>
       </c>
@@ -12966,7 +13491,7 @@
         <v>7.4409404207242801E-3</v>
       </c>
     </row>
-    <row r="334" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>4</v>
       </c>
@@ -12989,7 +13514,7 @@
         <v>7.5658724063938703E-3</v>
       </c>
     </row>
-    <row r="335" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>4</v>
       </c>
@@ -13012,7 +13537,7 @@
         <v>7.5384564403183996E-3</v>
       </c>
     </row>
-    <row r="336" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>4</v>
       </c>
@@ -16968,7 +17493,7 @@
         <v>2.6609797149656201E-3</v>
       </c>
     </row>
-    <row r="508" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A508">
         <v>5</v>
       </c>
@@ -16991,7 +17516,7 @@
         <v>2.4833811664435601E-3</v>
       </c>
     </row>
-    <row r="509" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A509">
         <v>5</v>
       </c>
@@ -17014,7 +17539,7 @@
         <v>2.7292891342774201E-3</v>
       </c>
     </row>
-    <row r="510" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A510">
         <v>5</v>
       </c>
@@ -17037,7 +17562,7 @@
         <v>2.7268116910085299E-3</v>
       </c>
     </row>
-    <row r="511" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A511">
         <v>5</v>
       </c>
@@ -17060,7 +17585,7 @@
         <v>2.7669014720134101E-3</v>
       </c>
     </row>
-    <row r="512" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A512">
         <v>5</v>
       </c>
@@ -17083,7 +17608,7 @@
         <v>2.6011830477933998E-3</v>
       </c>
     </row>
-    <row r="513" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A513">
         <v>5</v>
       </c>
@@ -17106,7 +17631,7 @@
         <v>2.55062291485797E-3</v>
       </c>
     </row>
-    <row r="514" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A514">
         <v>5</v>
       </c>
@@ -20648,7 +21173,7 @@
         <v>3.21038254301279E-3</v>
       </c>
     </row>
-    <row r="668" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="668" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A668">
         <v>6</v>
       </c>
@@ -20671,7 +21196,7 @@
         <v>1.9434915309188699E-3</v>
       </c>
     </row>
-    <row r="669" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="669" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A669">
         <v>6</v>
       </c>
@@ -20694,7 +21219,7 @@
         <v>2.7498611449181302E-3</v>
       </c>
     </row>
-    <row r="670" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="670" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A670">
         <v>6</v>
       </c>
@@ -20717,7 +21242,7 @@
         <v>2.3289703212294802E-3</v>
       </c>
     </row>
-    <row r="671" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="671" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A671">
         <v>6</v>
       </c>
@@ -20740,7 +21265,7 @@
         <v>2.2770086035823699E-3</v>
       </c>
     </row>
-    <row r="672" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="672" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A672">
         <v>6</v>
       </c>
@@ -20763,7 +21288,7 @@
         <v>2.4598174162356701E-3</v>
       </c>
     </row>
-    <row r="673" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="673" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A673">
         <v>6</v>
       </c>
@@ -20786,7 +21311,7 @@
         <v>2.4102575367566598E-3</v>
       </c>
     </row>
-    <row r="674" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="674" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A674">
         <v>6</v>
       </c>
@@ -20809,7 +21334,7 @@
         <v>2.34677540763079E-3</v>
       </c>
     </row>
-    <row r="675" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="675" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A675">
         <v>6</v>
       </c>
@@ -20832,7 +21357,7 @@
         <v>2.3811332888433998E-3</v>
       </c>
     </row>
-    <row r="676" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="676" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A676">
         <v>6</v>
       </c>
@@ -20855,7 +21380,7 @@
         <v>2.3302614745597801E-3</v>
       </c>
     </row>
-    <row r="677" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="677" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A677">
         <v>6</v>
       </c>
@@ -20878,7 +21403,7 @@
         <v>2.7303955447713999E-3</v>
       </c>
     </row>
-    <row r="678" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="678" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A678">
         <v>6</v>
       </c>
@@ -24581,7 +25106,7 @@
         <v>1.0837007402291101E-2</v>
       </c>
     </row>
-    <row r="839" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="839" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A839">
         <v>7</v>
       </c>
@@ -24604,7 +25129,7 @@
         <v>2.0588777414662098E-3</v>
       </c>
     </row>
-    <row r="840" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="840" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A840">
         <v>7</v>
       </c>
@@ -24627,7 +25152,7 @@
         <v>2.45047131243577E-3</v>
       </c>
     </row>
-    <row r="841" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="841" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A841">
         <v>7</v>
       </c>
@@ -24650,7 +25175,7 @@
         <v>1.8353179009032499E-3</v>
       </c>
     </row>
-    <row r="842" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="842" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A842">
         <v>7</v>
       </c>
@@ -24673,7 +25198,7 @@
         <v>2.1789677792023801E-3</v>
       </c>
     </row>
-    <row r="843" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="843" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A843">
         <v>7</v>
       </c>
@@ -24696,7 +25221,7 @@
         <v>2.1934291661862299E-3</v>
       </c>
     </row>
-    <row r="844" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="844" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A844">
         <v>7</v>
       </c>
@@ -24719,7 +25244,7 @@
         <v>2.0125646828548002E-3</v>
       </c>
     </row>
-    <row r="845" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="845" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A845">
         <v>7</v>
       </c>
@@ -24742,7 +25267,7 @@
         <v>2.2881037561553602E-3</v>
       </c>
     </row>
-    <row r="846" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="846" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A846">
         <v>7</v>
       </c>
@@ -24765,7 +25290,7 @@
         <v>1.90670118082883E-3</v>
       </c>
     </row>
-    <row r="847" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="847" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A847">
         <v>7</v>
       </c>
@@ -24788,7 +25313,7 @@
         <v>1.9307306676074601E-3</v>
       </c>
     </row>
-    <row r="848" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="848" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A848">
         <v>7</v>
       </c>
@@ -24811,7 +25336,7 @@
         <v>1.9386117775457201E-3</v>
       </c>
     </row>
-    <row r="849" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="849" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A849">
         <v>7</v>
       </c>
@@ -28767,7 +29292,7 @@
         <v>2.4646327867034901E-3</v>
       </c>
     </row>
-    <row r="1021" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1021" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1021">
         <v>8</v>
       </c>
@@ -28790,7 +29315,7 @@
         <v>2.57806011620178E-3</v>
       </c>
     </row>
-    <row r="1022" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1022" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1022">
         <v>8</v>
       </c>
@@ -28813,7 +29338,7 @@
         <v>2.2502931886244498E-3</v>
       </c>
     </row>
-    <row r="1023" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1023" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1023">
         <v>8</v>
       </c>
@@ -28836,7 +29361,7 @@
         <v>2.1022462504474899E-3</v>
       </c>
     </row>
-    <row r="1024" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1024" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1024">
         <v>8</v>
       </c>
@@ -28859,7 +29384,7 @@
         <v>2.11961227554152E-3</v>
       </c>
     </row>
-    <row r="1025" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1025" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1025">
         <v>8</v>
       </c>
@@ -28882,7 +29407,7 @@
         <v>1.9904699644612799E-3</v>
       </c>
     </row>
-    <row r="1026" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1026" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1026">
         <v>8</v>
       </c>
@@ -28905,7 +29430,7 @@
         <v>2.0501220841233699E-3</v>
       </c>
     </row>
-    <row r="1027" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1027" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1027">
         <v>8</v>
       </c>
@@ -32447,7 +32972,7 @@
         <v>6.5613566642227497E-3</v>
       </c>
     </row>
-    <row r="1181" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1181">
         <v>9</v>
       </c>
@@ -32470,7 +32995,7 @@
         <v>8.5183541028838999E-3</v>
       </c>
     </row>
-    <row r="1182" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1182">
         <v>9</v>
       </c>
@@ -32493,7 +33018,7 @@
         <v>7.8991808626816193E-3</v>
       </c>
     </row>
-    <row r="1183" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1183">
         <v>9</v>
       </c>
@@ -32516,7 +33041,7 @@
         <v>6.1349413052430302E-3</v>
       </c>
     </row>
-    <row r="1184" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1184">
         <v>9</v>
       </c>
@@ -32539,7 +33064,7 @@
         <v>7.64986617971849E-3</v>
       </c>
     </row>
-    <row r="1185" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1185">
         <v>9</v>
       </c>
@@ -32562,7 +33087,7 @@
         <v>8.2558595242717796E-3</v>
       </c>
     </row>
-    <row r="1186" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1186">
         <v>9</v>
       </c>
@@ -32585,7 +33110,7 @@
         <v>7.3250578022593304E-3</v>
       </c>
     </row>
-    <row r="1187" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1187">
         <v>9</v>
       </c>
@@ -32608,7 +33133,7 @@
         <v>6.71346599303456E-3</v>
       </c>
     </row>
-    <row r="1188" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1188">
         <v>9</v>
       </c>
@@ -32631,7 +33156,7 @@
         <v>6.8098884324581301E-3</v>
       </c>
     </row>
-    <row r="1189" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1189">
         <v>9</v>
       </c>
@@ -32654,7 +33179,7 @@
         <v>6.4516661615481204E-3</v>
       </c>
     </row>
-    <row r="1190" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1190">
         <v>9</v>
       </c>
@@ -32677,7 +33202,7 @@
         <v>6.6909209631000202E-3</v>
       </c>
     </row>
-    <row r="1191" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1191">
         <v>9</v>
       </c>
@@ -36380,7 +36905,7 @@
         <v>1.7760012697529901E-2</v>
       </c>
     </row>
-    <row r="1352" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1352" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1352">
         <v>10</v>
       </c>
@@ -36403,7 +36928,7 @@
         <v>4.61830742097534E-3</v>
       </c>
     </row>
-    <row r="1353" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1353" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1353">
         <v>10</v>
       </c>
@@ -36426,7 +36951,7 @@
         <v>4.9670892352521598E-3</v>
       </c>
     </row>
-    <row r="1354" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1354" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1354">
         <v>10</v>
       </c>
@@ -36449,7 +36974,7 @@
         <v>4.7999666577677102E-3</v>
       </c>
     </row>
-    <row r="1355" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1355" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1355">
         <v>10</v>
       </c>
@@ -36472,7 +36997,7 @@
         <v>4.3933521575185101E-3</v>
       </c>
     </row>
-    <row r="1356" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1356" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1356">
         <v>10</v>
       </c>
@@ -36495,7 +37020,7 @@
         <v>4.5105543196721698E-3</v>
       </c>
     </row>
-    <row r="1357" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1357" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1357">
         <v>10</v>
       </c>
@@ -36518,7 +37043,7 @@
         <v>4.3480779243237604E-3</v>
       </c>
     </row>
-    <row r="1358" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1358" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1358">
         <v>10</v>
       </c>
@@ -36541,7 +37066,7 @@
         <v>4.0013908265737804E-3</v>
       </c>
     </row>
-    <row r="1359" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1359" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1359">
         <v>10</v>
       </c>
@@ -36564,7 +37089,7 @@
         <v>3.7995531353189199E-3</v>
       </c>
     </row>
-    <row r="1360" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1360" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1360">
         <v>10</v>
       </c>
@@ -36587,7 +37112,7 @@
         <v>4.0485115449161698E-3</v>
       </c>
     </row>
-    <row r="1361" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1361" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1361">
         <v>10</v>
       </c>
@@ -36610,7 +37135,7 @@
         <v>4.2317323315029399E-3</v>
       </c>
     </row>
-    <row r="1362" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1362" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1362">
         <v>10</v>
       </c>
@@ -40567,17 +41092,25 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1533">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="11"/>
-        <filter val="5"/>
-        <filter val="8"/>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="A1:G1533" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
         <filter val="20"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="10"/>
+        <filter val="11"/>
+        <filter val="12"/>
+        <filter val="2"/>
+        <filter val="3"/>
+        <filter val="4"/>
+        <filter val="5"/>
+        <filter val="6"/>
+        <filter val="7"/>
+        <filter val="8"/>
+        <filter val="9"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>